<commit_message>
Cleaned and reorgnized files
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\stock_price_crawler\stock-price-crawler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1E12A1-4FD3-4A2B-9305-9F23585FA71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436EF275-92BE-4F63-9C42-EDC5F27E34A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>symbol</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>RBF263.CF(RBC U.S. Equity Fund Series A)</t>
+  </si>
+  <si>
+    <t>RBF590.CF(RBC U.S. Dividend Fund Series A)</t>
+  </si>
+  <si>
+    <t>RBF557.CF(RBC U.S. Index Fund Series Dz)</t>
+  </si>
+  <si>
+    <t>INA48603.CF(IA US Daq Index (Ia) SRP7575Myed+)</t>
+  </si>
+  <si>
+    <t>INA36081.CF(iA Global Innovators Fid SRP75100)</t>
+  </si>
+  <si>
+    <t>AAPL(Apple Inc. (AAPL))</t>
+  </si>
+  <si>
+    <t>META(Meta Platforms, Inc. (META))</t>
+  </si>
+  <si>
+    <t>NVDA(NVIDIA Corporation (NVDA))</t>
+  </si>
+  <si>
+    <t>AMZN(Amazon.com, Inc. (AMZN))</t>
+  </si>
+  <si>
+    <t>MSFT(Microsoft Corporation (MSFT))</t>
+  </si>
+  <si>
+    <t>SHOP(Shopify Inc. (SHOP))</t>
+  </si>
+  <si>
+    <t>TSLA(Tesla, Inc. (TSLA))</t>
+  </si>
+  <si>
+    <t>GOOG(Alphabet Inc. (GOOG))</t>
+  </si>
+  <si>
+    <t>AVGO(Broadcom Inc. (AVGO))</t>
   </si>
 </sst>
 </file>
@@ -41,17 +80,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -72,16 +111,16 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -89,10 +128,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -396,25 +438,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>